<commit_message>
Modified YPS Lean Canvas.xlsx
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Lean Canvas.xlsx
+++ b/Business Plan Documents/YPS Lean Canvas.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>LEAN CANVAS</t>
   </si>
@@ -55,255 +54,6 @@
   </si>
   <si>
     <t>REVENUE STREAMS</t>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I have difficulty in identifying what to wear each day because:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I don’t have the time to prepare </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I don’t feel confident with their fashion sense</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I find engaging fashion as *luxurious* and expensive</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I find it hard to identify clothing that will match their physique (e.g. Those with physical qualities that are hard to pair with clothing)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I find it hard to dress in various themes for different occasions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I don’t want to shop online because I cannot use style as a filter to find clothing</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I do not want to shop online because I cannot physically see how the dress / the item would look *on me*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I feel intimidated with expensive items in shops that have unfamiliar and/or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>established</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> names</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>I don’t know if the shop / the mall has my size or the design that I want</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">
@@ -316,6 +66,23 @@
   <si>
     <t xml:space="preserve">A Mobile application that users can access anytime anywhere that will let you have your virtual wardrobe and as well as your personal stylist  that will guide users on how to mix and match clothes based on 
 their body features (e.g. Skin tone, body built and vital statistics ).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our Mobile Application is user friendly and can be accessed anytime,
+ anywhere through smartphones
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First mobile Application for Fashion that allows user to create a virtual wardrobe of their own closet and have access to different items of clothing brands such as Bench and Penshoppe and have a virtual fitting of the clothes to see if it fits them while the mobile application generates set of clothes that suits the users body features for suggestions.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Mostly but not limited to females and teenagers
+• Those who download applications specifically for the option of having a better fashion sense
+• Those who prefer selecting their clothing based on style and their measurements as a filter
+• Those who are also willing to pay a certain amount to be able to have a way to select clothing styles and purchase online
+• Clothing Brands and Online Boutiques
 </t>
   </si>
   <si>
@@ -339,22 +106,17 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-- Online boutiques ( Small/ Starting up online clothing shops that are affordable)
-- Clothing Brands (e.g. Bench, Penshoppe, and Oxygen)
+• Online boutiques ( Small/ Starting up online clothing shops that are affordable)
+• Clothing Brands (e.g. Bench, Penshoppe, and Oxygen)
 </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Our Mobile Application is user friendly and can be accessed anytime,
- anywhere through smartphones
-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,89 +147,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFD9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -530,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -707,52 +393,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF70AD47"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF70AD47"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF70AD47"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF70AD47"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA8D08D"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA8D08D"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA8D08D"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA8D08D"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA8D08D"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA8D08D"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -778,16 +423,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -808,33 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -847,59 +459,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,14 +819,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -1225,232 +837,236 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="28" t="s">
-        <v>24</v>
+      <c r="A16" s="19"/>
+      <c r="B16" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="10"/>
+      <c r="E16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="10"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="10"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="10"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="11"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="46"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -1536,82 +1152,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
-  <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="242.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="138.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="190.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="190.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="276.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-    </row>
-    <row r="9" spans="1:1" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="347.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A7:A8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified YPS Lean Canvas.xlsx to add cost structure
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Lean Canvas.xlsx
+++ b/Business Plan Documents/YPS Lean Canvas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>LEAN CANVAS</t>
   </si>
@@ -119,12 +119,118 @@
 • User’s subscription of Upgrade wardrobe capacity
 </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-implementation:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• Leasehold Improvements
+• Capital Equipment
+• Location / Admin Expenses
+• Advertising / Promo Expenses
+• Pre-opening salaries</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>During implementation:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• Monthly Salaries Expense
+• Advertising ( through social Media)
+• Interest expense
+• Depreciation Expense
+• Transportation
+• Monthly Utilities ( internet, water, electricity)
+• Monthly rental fee
+• Office supplies
+• Maintenance and Support</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +261,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="21">
     <fill>
@@ -456,10 +576,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,9 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -647,9 +765,19 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,9 +1068,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:F35"/>
     </sheetView>
   </sheetViews>
@@ -1199,78 +1327,96 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="62" t="s">
+      <c r="A27" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="54"/>
-      <c r="F27" s="55"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="58"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="57"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="57"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="58"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="58"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57"/>
+    </row>
+    <row r="35" spans="1:6" ht="155.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="50"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="60"/>
+    </row>
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="62"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="62"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="62"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="63"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>